<commit_message>
Include option for non registered members
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -5674,7 +5674,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5759,27 +5759,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5901,9 +5881,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="5.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="5.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6952,19 +6932,19 @@
       <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="6.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="6.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="6.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="6.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8456,18 +8436,18 @@
   <dimension ref="A1:Y1015"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="C168" activeCellId="0" sqref="C168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="6.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="6.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="6.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13741,21 +13721,21 @@
   </sheetPr>
   <dimension ref="A1:Y761"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="6.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="5.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="6.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31456,17 +31436,17 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="5.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="5.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32599,17 +32579,17 @@
   </sheetPr>
   <dimension ref="A1:AMJ496"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A484" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C493" activeCellId="0" sqref="C493"/>
+      <selection pane="bottomLeft" activeCell="D126" activeCellId="0" sqref="D126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.9375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="22.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="6.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="21.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="6.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41442,44 +41422,1042 @@
       <c r="AMI493" s="0"/>
       <c r="AMJ493" s="0"/>
     </row>
-    <row r="494" s="23" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A494" s="21" t="s">
+    <row r="494" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A494" s="20" t="s">
         <v>1810</v>
       </c>
-      <c r="B494" s="22" t="s">
+      <c r="B494" s="16" t="s">
         <v>1811</v>
       </c>
-      <c r="C494" s="22" t="s">
+      <c r="C494" s="16" t="s">
         <v>1812</v>
       </c>
-      <c r="D494" s="22" t="s">
+      <c r="D494" s="16" t="s">
         <v>1813</v>
       </c>
-      <c r="E494" s="21"/>
-      <c r="F494" s="21"/>
-      <c r="G494" s="21"/>
-      <c r="H494" s="21"/>
-      <c r="I494" s="21"/>
-      <c r="J494" s="21"/>
-      <c r="K494" s="21"/>
-      <c r="L494" s="21"/>
-      <c r="M494" s="21"/>
-      <c r="N494" s="21"/>
-      <c r="O494" s="21"/>
-      <c r="P494" s="21"/>
-      <c r="Q494" s="21"/>
-      <c r="R494" s="21"/>
-      <c r="S494" s="21"/>
-      <c r="T494" s="21"/>
-      <c r="U494" s="21"/>
-      <c r="V494" s="21"/>
-      <c r="W494" s="21"/>
-      <c r="X494" s="21"/>
-      <c r="Y494" s="21"/>
-      <c r="Z494" s="21"/>
+      <c r="E494" s="20"/>
+      <c r="F494" s="20"/>
+      <c r="G494" s="20"/>
+      <c r="H494" s="20"/>
+      <c r="I494" s="20"/>
+      <c r="J494" s="20"/>
+      <c r="K494" s="20"/>
+      <c r="L494" s="20"/>
+      <c r="M494" s="20"/>
+      <c r="N494" s="20"/>
+      <c r="O494" s="20"/>
+      <c r="P494" s="20"/>
+      <c r="Q494" s="20"/>
+      <c r="R494" s="20"/>
+      <c r="S494" s="20"/>
+      <c r="T494" s="20"/>
+      <c r="U494" s="20"/>
+      <c r="V494" s="20"/>
+      <c r="W494" s="20"/>
+      <c r="X494" s="20"/>
+      <c r="Y494" s="20"/>
+      <c r="Z494" s="20"/>
+      <c r="AA494" s="0"/>
+      <c r="AB494" s="0"/>
+      <c r="AC494" s="0"/>
+      <c r="AD494" s="0"/>
+      <c r="AE494" s="0"/>
+      <c r="AF494" s="0"/>
+      <c r="AG494" s="0"/>
+      <c r="AH494" s="0"/>
+      <c r="AI494" s="0"/>
+      <c r="AJ494" s="0"/>
+      <c r="AK494" s="0"/>
+      <c r="AL494" s="0"/>
+      <c r="AM494" s="0"/>
+      <c r="AN494" s="0"/>
+      <c r="AO494" s="0"/>
+      <c r="AP494" s="0"/>
+      <c r="AQ494" s="0"/>
+      <c r="AR494" s="0"/>
+      <c r="AS494" s="0"/>
+      <c r="AT494" s="0"/>
+      <c r="AU494" s="0"/>
+      <c r="AV494" s="0"/>
+      <c r="AW494" s="0"/>
+      <c r="AX494" s="0"/>
+      <c r="AY494" s="0"/>
+      <c r="AZ494" s="0"/>
+      <c r="BA494" s="0"/>
+      <c r="BB494" s="0"/>
+      <c r="BC494" s="0"/>
+      <c r="BD494" s="0"/>
+      <c r="BE494" s="0"/>
+      <c r="BF494" s="0"/>
+      <c r="BG494" s="0"/>
+      <c r="BH494" s="0"/>
+      <c r="BI494" s="0"/>
+      <c r="BJ494" s="0"/>
+      <c r="BK494" s="0"/>
+      <c r="BL494" s="0"/>
+      <c r="BM494" s="0"/>
+      <c r="BN494" s="0"/>
+      <c r="BO494" s="0"/>
+      <c r="BP494" s="0"/>
+      <c r="BQ494" s="0"/>
+      <c r="BR494" s="0"/>
+      <c r="BS494" s="0"/>
+      <c r="BT494" s="0"/>
+      <c r="BU494" s="0"/>
+      <c r="BV494" s="0"/>
+      <c r="BW494" s="0"/>
+      <c r="BX494" s="0"/>
+      <c r="BY494" s="0"/>
+      <c r="BZ494" s="0"/>
+      <c r="CA494" s="0"/>
+      <c r="CB494" s="0"/>
+      <c r="CC494" s="0"/>
+      <c r="CD494" s="0"/>
+      <c r="CE494" s="0"/>
+      <c r="CF494" s="0"/>
+      <c r="CG494" s="0"/>
+      <c r="CH494" s="0"/>
+      <c r="CI494" s="0"/>
+      <c r="CJ494" s="0"/>
+      <c r="CK494" s="0"/>
+      <c r="CL494" s="0"/>
+      <c r="CM494" s="0"/>
+      <c r="CN494" s="0"/>
+      <c r="CO494" s="0"/>
+      <c r="CP494" s="0"/>
+      <c r="CQ494" s="0"/>
+      <c r="CR494" s="0"/>
+      <c r="CS494" s="0"/>
+      <c r="CT494" s="0"/>
+      <c r="CU494" s="0"/>
+      <c r="CV494" s="0"/>
+      <c r="CW494" s="0"/>
+      <c r="CX494" s="0"/>
+      <c r="CY494" s="0"/>
+      <c r="CZ494" s="0"/>
+      <c r="DA494" s="0"/>
+      <c r="DB494" s="0"/>
+      <c r="DC494" s="0"/>
+      <c r="DD494" s="0"/>
+      <c r="DE494" s="0"/>
+      <c r="DF494" s="0"/>
+      <c r="DG494" s="0"/>
+      <c r="DH494" s="0"/>
+      <c r="DI494" s="0"/>
+      <c r="DJ494" s="0"/>
+      <c r="DK494" s="0"/>
+      <c r="DL494" s="0"/>
+      <c r="DM494" s="0"/>
+      <c r="DN494" s="0"/>
+      <c r="DO494" s="0"/>
+      <c r="DP494" s="0"/>
+      <c r="DQ494" s="0"/>
+      <c r="DR494" s="0"/>
+      <c r="DS494" s="0"/>
+      <c r="DT494" s="0"/>
+      <c r="DU494" s="0"/>
+      <c r="DV494" s="0"/>
+      <c r="DW494" s="0"/>
+      <c r="DX494" s="0"/>
+      <c r="DY494" s="0"/>
+      <c r="DZ494" s="0"/>
+      <c r="EA494" s="0"/>
+      <c r="EB494" s="0"/>
+      <c r="EC494" s="0"/>
+      <c r="ED494" s="0"/>
+      <c r="EE494" s="0"/>
+      <c r="EF494" s="0"/>
+      <c r="EG494" s="0"/>
+      <c r="EH494" s="0"/>
+      <c r="EI494" s="0"/>
+      <c r="EJ494" s="0"/>
+      <c r="EK494" s="0"/>
+      <c r="EL494" s="0"/>
+      <c r="EM494" s="0"/>
+      <c r="EN494" s="0"/>
+      <c r="EO494" s="0"/>
+      <c r="EP494" s="0"/>
+      <c r="EQ494" s="0"/>
+      <c r="ER494" s="0"/>
+      <c r="ES494" s="0"/>
+      <c r="ET494" s="0"/>
+      <c r="EU494" s="0"/>
+      <c r="EV494" s="0"/>
+      <c r="EW494" s="0"/>
+      <c r="EX494" s="0"/>
+      <c r="EY494" s="0"/>
+      <c r="EZ494" s="0"/>
+      <c r="FA494" s="0"/>
+      <c r="FB494" s="0"/>
+      <c r="FC494" s="0"/>
+      <c r="FD494" s="0"/>
+      <c r="FE494" s="0"/>
+      <c r="FF494" s="0"/>
+      <c r="FG494" s="0"/>
+      <c r="FH494" s="0"/>
+      <c r="FI494" s="0"/>
+      <c r="FJ494" s="0"/>
+      <c r="FK494" s="0"/>
+      <c r="FL494" s="0"/>
+      <c r="FM494" s="0"/>
+      <c r="FN494" s="0"/>
+      <c r="FO494" s="0"/>
+      <c r="FP494" s="0"/>
+      <c r="FQ494" s="0"/>
+      <c r="FR494" s="0"/>
+      <c r="FS494" s="0"/>
+      <c r="FT494" s="0"/>
+      <c r="FU494" s="0"/>
+      <c r="FV494" s="0"/>
+      <c r="FW494" s="0"/>
+      <c r="FX494" s="0"/>
+      <c r="FY494" s="0"/>
+      <c r="FZ494" s="0"/>
+      <c r="GA494" s="0"/>
+      <c r="GB494" s="0"/>
+      <c r="GC494" s="0"/>
+      <c r="GD494" s="0"/>
+      <c r="GE494" s="0"/>
+      <c r="GF494" s="0"/>
+      <c r="GG494" s="0"/>
+      <c r="GH494" s="0"/>
+      <c r="GI494" s="0"/>
+      <c r="GJ494" s="0"/>
+      <c r="GK494" s="0"/>
+      <c r="GL494" s="0"/>
+      <c r="GM494" s="0"/>
+      <c r="GN494" s="0"/>
+      <c r="GO494" s="0"/>
+      <c r="GP494" s="0"/>
+      <c r="GQ494" s="0"/>
+      <c r="GR494" s="0"/>
+      <c r="GS494" s="0"/>
+      <c r="GT494" s="0"/>
+      <c r="GU494" s="0"/>
+      <c r="GV494" s="0"/>
+      <c r="GW494" s="0"/>
+      <c r="GX494" s="0"/>
+      <c r="GY494" s="0"/>
+      <c r="GZ494" s="0"/>
+      <c r="HA494" s="0"/>
+      <c r="HB494" s="0"/>
+      <c r="HC494" s="0"/>
+      <c r="HD494" s="0"/>
+      <c r="HE494" s="0"/>
+      <c r="HF494" s="0"/>
+      <c r="HG494" s="0"/>
+      <c r="HH494" s="0"/>
+      <c r="HI494" s="0"/>
+      <c r="HJ494" s="0"/>
+      <c r="HK494" s="0"/>
+      <c r="HL494" s="0"/>
+      <c r="HM494" s="0"/>
+      <c r="HN494" s="0"/>
+      <c r="HO494" s="0"/>
+      <c r="HP494" s="0"/>
+      <c r="HQ494" s="0"/>
+      <c r="HR494" s="0"/>
+      <c r="HS494" s="0"/>
+      <c r="HT494" s="0"/>
+      <c r="HU494" s="0"/>
+      <c r="HV494" s="0"/>
+      <c r="HW494" s="0"/>
+      <c r="HX494" s="0"/>
+      <c r="HY494" s="0"/>
+      <c r="HZ494" s="0"/>
+      <c r="IA494" s="0"/>
+      <c r="IB494" s="0"/>
+      <c r="IC494" s="0"/>
+      <c r="ID494" s="0"/>
+      <c r="IE494" s="0"/>
+      <c r="IF494" s="0"/>
+      <c r="IG494" s="0"/>
+      <c r="IH494" s="0"/>
+      <c r="II494" s="0"/>
+      <c r="IJ494" s="0"/>
+      <c r="IK494" s="0"/>
+      <c r="IL494" s="0"/>
+      <c r="IM494" s="0"/>
+      <c r="IN494" s="0"/>
+      <c r="IO494" s="0"/>
+      <c r="IP494" s="0"/>
+      <c r="IQ494" s="0"/>
+      <c r="IR494" s="0"/>
+      <c r="IS494" s="0"/>
+      <c r="IT494" s="0"/>
+      <c r="IU494" s="0"/>
+      <c r="IV494" s="0"/>
+      <c r="IW494" s="0"/>
+      <c r="IX494" s="0"/>
+      <c r="IY494" s="0"/>
+      <c r="IZ494" s="0"/>
+      <c r="JA494" s="0"/>
+      <c r="JB494" s="0"/>
+      <c r="JC494" s="0"/>
+      <c r="JD494" s="0"/>
+      <c r="JE494" s="0"/>
+      <c r="JF494" s="0"/>
+      <c r="JG494" s="0"/>
+      <c r="JH494" s="0"/>
+      <c r="JI494" s="0"/>
+      <c r="JJ494" s="0"/>
+      <c r="JK494" s="0"/>
+      <c r="JL494" s="0"/>
+      <c r="JM494" s="0"/>
+      <c r="JN494" s="0"/>
+      <c r="JO494" s="0"/>
+      <c r="JP494" s="0"/>
+      <c r="JQ494" s="0"/>
+      <c r="JR494" s="0"/>
+      <c r="JS494" s="0"/>
+      <c r="JT494" s="0"/>
+      <c r="JU494" s="0"/>
+      <c r="JV494" s="0"/>
+      <c r="JW494" s="0"/>
+      <c r="JX494" s="0"/>
+      <c r="JY494" s="0"/>
+      <c r="JZ494" s="0"/>
+      <c r="KA494" s="0"/>
+      <c r="KB494" s="0"/>
+      <c r="KC494" s="0"/>
+      <c r="KD494" s="0"/>
+      <c r="KE494" s="0"/>
+      <c r="KF494" s="0"/>
+      <c r="KG494" s="0"/>
+      <c r="KH494" s="0"/>
+      <c r="KI494" s="0"/>
+      <c r="KJ494" s="0"/>
+      <c r="KK494" s="0"/>
+      <c r="KL494" s="0"/>
+      <c r="KM494" s="0"/>
+      <c r="KN494" s="0"/>
+      <c r="KO494" s="0"/>
+      <c r="KP494" s="0"/>
+      <c r="KQ494" s="0"/>
+      <c r="KR494" s="0"/>
+      <c r="KS494" s="0"/>
+      <c r="KT494" s="0"/>
+      <c r="KU494" s="0"/>
+      <c r="KV494" s="0"/>
+      <c r="KW494" s="0"/>
+      <c r="KX494" s="0"/>
+      <c r="KY494" s="0"/>
+      <c r="KZ494" s="0"/>
+      <c r="LA494" s="0"/>
+      <c r="LB494" s="0"/>
+      <c r="LC494" s="0"/>
+      <c r="LD494" s="0"/>
+      <c r="LE494" s="0"/>
+      <c r="LF494" s="0"/>
+      <c r="LG494" s="0"/>
+      <c r="LH494" s="0"/>
+      <c r="LI494" s="0"/>
+      <c r="LJ494" s="0"/>
+      <c r="LK494" s="0"/>
+      <c r="LL494" s="0"/>
+      <c r="LM494" s="0"/>
+      <c r="LN494" s="0"/>
+      <c r="LO494" s="0"/>
+      <c r="LP494" s="0"/>
+      <c r="LQ494" s="0"/>
+      <c r="LR494" s="0"/>
+      <c r="LS494" s="0"/>
+      <c r="LT494" s="0"/>
+      <c r="LU494" s="0"/>
+      <c r="LV494" s="0"/>
+      <c r="LW494" s="0"/>
+      <c r="LX494" s="0"/>
+      <c r="LY494" s="0"/>
+      <c r="LZ494" s="0"/>
+      <c r="MA494" s="0"/>
+      <c r="MB494" s="0"/>
+      <c r="MC494" s="0"/>
+      <c r="MD494" s="0"/>
+      <c r="ME494" s="0"/>
+      <c r="MF494" s="0"/>
+      <c r="MG494" s="0"/>
+      <c r="MH494" s="0"/>
+      <c r="MI494" s="0"/>
+      <c r="MJ494" s="0"/>
+      <c r="MK494" s="0"/>
+      <c r="ML494" s="0"/>
+      <c r="MM494" s="0"/>
+      <c r="MN494" s="0"/>
+      <c r="MO494" s="0"/>
+      <c r="MP494" s="0"/>
+      <c r="MQ494" s="0"/>
+      <c r="MR494" s="0"/>
+      <c r="MS494" s="0"/>
+      <c r="MT494" s="0"/>
+      <c r="MU494" s="0"/>
+      <c r="MV494" s="0"/>
+      <c r="MW494" s="0"/>
+      <c r="MX494" s="0"/>
+      <c r="MY494" s="0"/>
+      <c r="MZ494" s="0"/>
+      <c r="NA494" s="0"/>
+      <c r="NB494" s="0"/>
+      <c r="NC494" s="0"/>
+      <c r="ND494" s="0"/>
+      <c r="NE494" s="0"/>
+      <c r="NF494" s="0"/>
+      <c r="NG494" s="0"/>
+      <c r="NH494" s="0"/>
+      <c r="NI494" s="0"/>
+      <c r="NJ494" s="0"/>
+      <c r="NK494" s="0"/>
+      <c r="NL494" s="0"/>
+      <c r="NM494" s="0"/>
+      <c r="NN494" s="0"/>
+      <c r="NO494" s="0"/>
+      <c r="NP494" s="0"/>
+      <c r="NQ494" s="0"/>
+      <c r="NR494" s="0"/>
+      <c r="NS494" s="0"/>
+      <c r="NT494" s="0"/>
+      <c r="NU494" s="0"/>
+      <c r="NV494" s="0"/>
+      <c r="NW494" s="0"/>
+      <c r="NX494" s="0"/>
+      <c r="NY494" s="0"/>
+      <c r="NZ494" s="0"/>
+      <c r="OA494" s="0"/>
+      <c r="OB494" s="0"/>
+      <c r="OC494" s="0"/>
+      <c r="OD494" s="0"/>
+      <c r="OE494" s="0"/>
+      <c r="OF494" s="0"/>
+      <c r="OG494" s="0"/>
+      <c r="OH494" s="0"/>
+      <c r="OI494" s="0"/>
+      <c r="OJ494" s="0"/>
+      <c r="OK494" s="0"/>
+      <c r="OL494" s="0"/>
+      <c r="OM494" s="0"/>
+      <c r="ON494" s="0"/>
+      <c r="OO494" s="0"/>
+      <c r="OP494" s="0"/>
+      <c r="OQ494" s="0"/>
+      <c r="OR494" s="0"/>
+      <c r="OS494" s="0"/>
+      <c r="OT494" s="0"/>
+      <c r="OU494" s="0"/>
+      <c r="OV494" s="0"/>
+      <c r="OW494" s="0"/>
+      <c r="OX494" s="0"/>
+      <c r="OY494" s="0"/>
+      <c r="OZ494" s="0"/>
+      <c r="PA494" s="0"/>
+      <c r="PB494" s="0"/>
+      <c r="PC494" s="0"/>
+      <c r="PD494" s="0"/>
+      <c r="PE494" s="0"/>
+      <c r="PF494" s="0"/>
+      <c r="PG494" s="0"/>
+      <c r="PH494" s="0"/>
+      <c r="PI494" s="0"/>
+      <c r="PJ494" s="0"/>
+      <c r="PK494" s="0"/>
+      <c r="PL494" s="0"/>
+      <c r="PM494" s="0"/>
+      <c r="PN494" s="0"/>
+      <c r="PO494" s="0"/>
+      <c r="PP494" s="0"/>
+      <c r="PQ494" s="0"/>
+      <c r="PR494" s="0"/>
+      <c r="PS494" s="0"/>
+      <c r="PT494" s="0"/>
+      <c r="PU494" s="0"/>
+      <c r="PV494" s="0"/>
+      <c r="PW494" s="0"/>
+      <c r="PX494" s="0"/>
+      <c r="PY494" s="0"/>
+      <c r="PZ494" s="0"/>
+      <c r="QA494" s="0"/>
+      <c r="QB494" s="0"/>
+      <c r="QC494" s="0"/>
+      <c r="QD494" s="0"/>
+      <c r="QE494" s="0"/>
+      <c r="QF494" s="0"/>
+      <c r="QG494" s="0"/>
+      <c r="QH494" s="0"/>
+      <c r="QI494" s="0"/>
+      <c r="QJ494" s="0"/>
+      <c r="QK494" s="0"/>
+      <c r="QL494" s="0"/>
+      <c r="QM494" s="0"/>
+      <c r="QN494" s="0"/>
+      <c r="QO494" s="0"/>
+      <c r="QP494" s="0"/>
+      <c r="QQ494" s="0"/>
+      <c r="QR494" s="0"/>
+      <c r="QS494" s="0"/>
+      <c r="QT494" s="0"/>
+      <c r="QU494" s="0"/>
+      <c r="QV494" s="0"/>
+      <c r="QW494" s="0"/>
+      <c r="QX494" s="0"/>
+      <c r="QY494" s="0"/>
+      <c r="QZ494" s="0"/>
+      <c r="RA494" s="0"/>
+      <c r="RB494" s="0"/>
+      <c r="RC494" s="0"/>
+      <c r="RD494" s="0"/>
+      <c r="RE494" s="0"/>
+      <c r="RF494" s="0"/>
+      <c r="RG494" s="0"/>
+      <c r="RH494" s="0"/>
+      <c r="RI494" s="0"/>
+      <c r="RJ494" s="0"/>
+      <c r="RK494" s="0"/>
+      <c r="RL494" s="0"/>
+      <c r="RM494" s="0"/>
+      <c r="RN494" s="0"/>
+      <c r="RO494" s="0"/>
+      <c r="RP494" s="0"/>
+      <c r="RQ494" s="0"/>
+      <c r="RR494" s="0"/>
+      <c r="RS494" s="0"/>
+      <c r="RT494" s="0"/>
+      <c r="RU494" s="0"/>
+      <c r="RV494" s="0"/>
+      <c r="RW494" s="0"/>
+      <c r="RX494" s="0"/>
+      <c r="RY494" s="0"/>
+      <c r="RZ494" s="0"/>
+      <c r="SA494" s="0"/>
+      <c r="SB494" s="0"/>
+      <c r="SC494" s="0"/>
+      <c r="SD494" s="0"/>
+      <c r="SE494" s="0"/>
+      <c r="SF494" s="0"/>
+      <c r="SG494" s="0"/>
+      <c r="SH494" s="0"/>
+      <c r="SI494" s="0"/>
+      <c r="SJ494" s="0"/>
+      <c r="SK494" s="0"/>
+      <c r="SL494" s="0"/>
+      <c r="SM494" s="0"/>
+      <c r="SN494" s="0"/>
+      <c r="SO494" s="0"/>
+      <c r="SP494" s="0"/>
+      <c r="SQ494" s="0"/>
+      <c r="SR494" s="0"/>
+      <c r="SS494" s="0"/>
+      <c r="ST494" s="0"/>
+      <c r="SU494" s="0"/>
+      <c r="SV494" s="0"/>
+      <c r="SW494" s="0"/>
+      <c r="SX494" s="0"/>
+      <c r="SY494" s="0"/>
+      <c r="SZ494" s="0"/>
+      <c r="TA494" s="0"/>
+      <c r="TB494" s="0"/>
+      <c r="TC494" s="0"/>
+      <c r="TD494" s="0"/>
+      <c r="TE494" s="0"/>
+      <c r="TF494" s="0"/>
+      <c r="TG494" s="0"/>
+      <c r="TH494" s="0"/>
+      <c r="TI494" s="0"/>
+      <c r="TJ494" s="0"/>
+      <c r="TK494" s="0"/>
+      <c r="TL494" s="0"/>
+      <c r="TM494" s="0"/>
+      <c r="TN494" s="0"/>
+      <c r="TO494" s="0"/>
+      <c r="TP494" s="0"/>
+      <c r="TQ494" s="0"/>
+      <c r="TR494" s="0"/>
+      <c r="TS494" s="0"/>
+      <c r="TT494" s="0"/>
+      <c r="TU494" s="0"/>
+      <c r="TV494" s="0"/>
+      <c r="TW494" s="0"/>
+      <c r="TX494" s="0"/>
+      <c r="TY494" s="0"/>
+      <c r="TZ494" s="0"/>
+      <c r="UA494" s="0"/>
+      <c r="UB494" s="0"/>
+      <c r="UC494" s="0"/>
+      <c r="UD494" s="0"/>
+      <c r="UE494" s="0"/>
+      <c r="UF494" s="0"/>
+      <c r="UG494" s="0"/>
+      <c r="UH494" s="0"/>
+      <c r="UI494" s="0"/>
+      <c r="UJ494" s="0"/>
+      <c r="UK494" s="0"/>
+      <c r="UL494" s="0"/>
+      <c r="UM494" s="0"/>
+      <c r="UN494" s="0"/>
+      <c r="UO494" s="0"/>
+      <c r="UP494" s="0"/>
+      <c r="UQ494" s="0"/>
+      <c r="UR494" s="0"/>
+      <c r="US494" s="0"/>
+      <c r="UT494" s="0"/>
+      <c r="UU494" s="0"/>
+      <c r="UV494" s="0"/>
+      <c r="UW494" s="0"/>
+      <c r="UX494" s="0"/>
+      <c r="UY494" s="0"/>
+      <c r="UZ494" s="0"/>
+      <c r="VA494" s="0"/>
+      <c r="VB494" s="0"/>
+      <c r="VC494" s="0"/>
+      <c r="VD494" s="0"/>
+      <c r="VE494" s="0"/>
+      <c r="VF494" s="0"/>
+      <c r="VG494" s="0"/>
+      <c r="VH494" s="0"/>
+      <c r="VI494" s="0"/>
+      <c r="VJ494" s="0"/>
+      <c r="VK494" s="0"/>
+      <c r="VL494" s="0"/>
+      <c r="VM494" s="0"/>
+      <c r="VN494" s="0"/>
+      <c r="VO494" s="0"/>
+      <c r="VP494" s="0"/>
+      <c r="VQ494" s="0"/>
+      <c r="VR494" s="0"/>
+      <c r="VS494" s="0"/>
+      <c r="VT494" s="0"/>
+      <c r="VU494" s="0"/>
+      <c r="VV494" s="0"/>
+      <c r="VW494" s="0"/>
+      <c r="VX494" s="0"/>
+      <c r="VY494" s="0"/>
+      <c r="VZ494" s="0"/>
+      <c r="WA494" s="0"/>
+      <c r="WB494" s="0"/>
+      <c r="WC494" s="0"/>
+      <c r="WD494" s="0"/>
+      <c r="WE494" s="0"/>
+      <c r="WF494" s="0"/>
+      <c r="WG494" s="0"/>
+      <c r="WH494" s="0"/>
+      <c r="WI494" s="0"/>
+      <c r="WJ494" s="0"/>
+      <c r="WK494" s="0"/>
+      <c r="WL494" s="0"/>
+      <c r="WM494" s="0"/>
+      <c r="WN494" s="0"/>
+      <c r="WO494" s="0"/>
+      <c r="WP494" s="0"/>
+      <c r="WQ494" s="0"/>
+      <c r="WR494" s="0"/>
+      <c r="WS494" s="0"/>
+      <c r="WT494" s="0"/>
+      <c r="WU494" s="0"/>
+      <c r="WV494" s="0"/>
+      <c r="WW494" s="0"/>
+      <c r="WX494" s="0"/>
+      <c r="WY494" s="0"/>
+      <c r="WZ494" s="0"/>
+      <c r="XA494" s="0"/>
+      <c r="XB494" s="0"/>
+      <c r="XC494" s="0"/>
+      <c r="XD494" s="0"/>
+      <c r="XE494" s="0"/>
+      <c r="XF494" s="0"/>
+      <c r="XG494" s="0"/>
+      <c r="XH494" s="0"/>
+      <c r="XI494" s="0"/>
+      <c r="XJ494" s="0"/>
+      <c r="XK494" s="0"/>
+      <c r="XL494" s="0"/>
+      <c r="XM494" s="0"/>
+      <c r="XN494" s="0"/>
+      <c r="XO494" s="0"/>
+      <c r="XP494" s="0"/>
+      <c r="XQ494" s="0"/>
+      <c r="XR494" s="0"/>
+      <c r="XS494" s="0"/>
+      <c r="XT494" s="0"/>
+      <c r="XU494" s="0"/>
+      <c r="XV494" s="0"/>
+      <c r="XW494" s="0"/>
+      <c r="XX494" s="0"/>
+      <c r="XY494" s="0"/>
+      <c r="XZ494" s="0"/>
+      <c r="YA494" s="0"/>
+      <c r="YB494" s="0"/>
+      <c r="YC494" s="0"/>
+      <c r="YD494" s="0"/>
+      <c r="YE494" s="0"/>
+      <c r="YF494" s="0"/>
+      <c r="YG494" s="0"/>
+      <c r="YH494" s="0"/>
+      <c r="YI494" s="0"/>
+      <c r="YJ494" s="0"/>
+      <c r="YK494" s="0"/>
+      <c r="YL494" s="0"/>
+      <c r="YM494" s="0"/>
+      <c r="YN494" s="0"/>
+      <c r="YO494" s="0"/>
+      <c r="YP494" s="0"/>
+      <c r="YQ494" s="0"/>
+      <c r="YR494" s="0"/>
+      <c r="YS494" s="0"/>
+      <c r="YT494" s="0"/>
+      <c r="YU494" s="0"/>
+      <c r="YV494" s="0"/>
+      <c r="YW494" s="0"/>
+      <c r="YX494" s="0"/>
+      <c r="YY494" s="0"/>
+      <c r="YZ494" s="0"/>
+      <c r="ZA494" s="0"/>
+      <c r="ZB494" s="0"/>
+      <c r="ZC494" s="0"/>
+      <c r="ZD494" s="0"/>
+      <c r="ZE494" s="0"/>
+      <c r="ZF494" s="0"/>
+      <c r="ZG494" s="0"/>
+      <c r="ZH494" s="0"/>
+      <c r="ZI494" s="0"/>
+      <c r="ZJ494" s="0"/>
+      <c r="ZK494" s="0"/>
+      <c r="ZL494" s="0"/>
+      <c r="ZM494" s="0"/>
+      <c r="ZN494" s="0"/>
+      <c r="ZO494" s="0"/>
+      <c r="ZP494" s="0"/>
+      <c r="ZQ494" s="0"/>
+      <c r="ZR494" s="0"/>
+      <c r="ZS494" s="0"/>
+      <c r="ZT494" s="0"/>
+      <c r="ZU494" s="0"/>
+      <c r="ZV494" s="0"/>
+      <c r="ZW494" s="0"/>
+      <c r="ZX494" s="0"/>
+      <c r="ZY494" s="0"/>
+      <c r="ZZ494" s="0"/>
+      <c r="AAA494" s="0"/>
+      <c r="AAB494" s="0"/>
+      <c r="AAC494" s="0"/>
+      <c r="AAD494" s="0"/>
+      <c r="AAE494" s="0"/>
+      <c r="AAF494" s="0"/>
+      <c r="AAG494" s="0"/>
+      <c r="AAH494" s="0"/>
+      <c r="AAI494" s="0"/>
+      <c r="AAJ494" s="0"/>
+      <c r="AAK494" s="0"/>
+      <c r="AAL494" s="0"/>
+      <c r="AAM494" s="0"/>
+      <c r="AAN494" s="0"/>
+      <c r="AAO494" s="0"/>
+      <c r="AAP494" s="0"/>
+      <c r="AAQ494" s="0"/>
+      <c r="AAR494" s="0"/>
+      <c r="AAS494" s="0"/>
+      <c r="AAT494" s="0"/>
+      <c r="AAU494" s="0"/>
+      <c r="AAV494" s="0"/>
+      <c r="AAW494" s="0"/>
+      <c r="AAX494" s="0"/>
+      <c r="AAY494" s="0"/>
+      <c r="AAZ494" s="0"/>
+      <c r="ABA494" s="0"/>
+      <c r="ABB494" s="0"/>
+      <c r="ABC494" s="0"/>
+      <c r="ABD494" s="0"/>
+      <c r="ABE494" s="0"/>
+      <c r="ABF494" s="0"/>
+      <c r="ABG494" s="0"/>
+      <c r="ABH494" s="0"/>
+      <c r="ABI494" s="0"/>
+      <c r="ABJ494" s="0"/>
+      <c r="ABK494" s="0"/>
+      <c r="ABL494" s="0"/>
+      <c r="ABM494" s="0"/>
+      <c r="ABN494" s="0"/>
+      <c r="ABO494" s="0"/>
+      <c r="ABP494" s="0"/>
+      <c r="ABQ494" s="0"/>
+      <c r="ABR494" s="0"/>
+      <c r="ABS494" s="0"/>
+      <c r="ABT494" s="0"/>
+      <c r="ABU494" s="0"/>
+      <c r="ABV494" s="0"/>
+      <c r="ABW494" s="0"/>
+      <c r="ABX494" s="0"/>
+      <c r="ABY494" s="0"/>
+      <c r="ABZ494" s="0"/>
+      <c r="ACA494" s="0"/>
+      <c r="ACB494" s="0"/>
+      <c r="ACC494" s="0"/>
+      <c r="ACD494" s="0"/>
+      <c r="ACE494" s="0"/>
+      <c r="ACF494" s="0"/>
+      <c r="ACG494" s="0"/>
+      <c r="ACH494" s="0"/>
+      <c r="ACI494" s="0"/>
+      <c r="ACJ494" s="0"/>
+      <c r="ACK494" s="0"/>
+      <c r="ACL494" s="0"/>
+      <c r="ACM494" s="0"/>
+      <c r="ACN494" s="0"/>
+      <c r="ACO494" s="0"/>
+      <c r="ACP494" s="0"/>
+      <c r="ACQ494" s="0"/>
+      <c r="ACR494" s="0"/>
+      <c r="ACS494" s="0"/>
+      <c r="ACT494" s="0"/>
+      <c r="ACU494" s="0"/>
+      <c r="ACV494" s="0"/>
+      <c r="ACW494" s="0"/>
+      <c r="ACX494" s="0"/>
+      <c r="ACY494" s="0"/>
+      <c r="ACZ494" s="0"/>
+      <c r="ADA494" s="0"/>
+      <c r="ADB494" s="0"/>
+      <c r="ADC494" s="0"/>
+      <c r="ADD494" s="0"/>
+      <c r="ADE494" s="0"/>
+      <c r="ADF494" s="0"/>
+      <c r="ADG494" s="0"/>
+      <c r="ADH494" s="0"/>
+      <c r="ADI494" s="0"/>
+      <c r="ADJ494" s="0"/>
+      <c r="ADK494" s="0"/>
+      <c r="ADL494" s="0"/>
+      <c r="ADM494" s="0"/>
+      <c r="ADN494" s="0"/>
+      <c r="ADO494" s="0"/>
+      <c r="ADP494" s="0"/>
+      <c r="ADQ494" s="0"/>
+      <c r="ADR494" s="0"/>
+      <c r="ADS494" s="0"/>
+      <c r="ADT494" s="0"/>
+      <c r="ADU494" s="0"/>
+      <c r="ADV494" s="0"/>
+      <c r="ADW494" s="0"/>
+      <c r="ADX494" s="0"/>
+      <c r="ADY494" s="0"/>
+      <c r="ADZ494" s="0"/>
+      <c r="AEA494" s="0"/>
+      <c r="AEB494" s="0"/>
+      <c r="AEC494" s="0"/>
+      <c r="AED494" s="0"/>
+      <c r="AEE494" s="0"/>
+      <c r="AEF494" s="0"/>
+      <c r="AEG494" s="0"/>
+      <c r="AEH494" s="0"/>
+      <c r="AEI494" s="0"/>
+      <c r="AEJ494" s="0"/>
+      <c r="AEK494" s="0"/>
+      <c r="AEL494" s="0"/>
+      <c r="AEM494" s="0"/>
+      <c r="AEN494" s="0"/>
+      <c r="AEO494" s="0"/>
+      <c r="AEP494" s="0"/>
+      <c r="AEQ494" s="0"/>
+      <c r="AER494" s="0"/>
+      <c r="AES494" s="0"/>
+      <c r="AET494" s="0"/>
+      <c r="AEU494" s="0"/>
+      <c r="AEV494" s="0"/>
+      <c r="AEW494" s="0"/>
+      <c r="AEX494" s="0"/>
+      <c r="AEY494" s="0"/>
+      <c r="AEZ494" s="0"/>
+      <c r="AFA494" s="0"/>
+      <c r="AFB494" s="0"/>
+      <c r="AFC494" s="0"/>
+      <c r="AFD494" s="0"/>
+      <c r="AFE494" s="0"/>
+      <c r="AFF494" s="0"/>
+      <c r="AFG494" s="0"/>
+      <c r="AFH494" s="0"/>
+      <c r="AFI494" s="0"/>
+      <c r="AFJ494" s="0"/>
+      <c r="AFK494" s="0"/>
+      <c r="AFL494" s="0"/>
+      <c r="AFM494" s="0"/>
+      <c r="AFN494" s="0"/>
+      <c r="AFO494" s="0"/>
+      <c r="AFP494" s="0"/>
+      <c r="AFQ494" s="0"/>
+      <c r="AFR494" s="0"/>
+      <c r="AFS494" s="0"/>
+      <c r="AFT494" s="0"/>
+      <c r="AFU494" s="0"/>
+      <c r="AFV494" s="0"/>
+      <c r="AFW494" s="0"/>
+      <c r="AFX494" s="0"/>
+      <c r="AFY494" s="0"/>
+      <c r="AFZ494" s="0"/>
+      <c r="AGA494" s="0"/>
+      <c r="AGB494" s="0"/>
+      <c r="AGC494" s="0"/>
+      <c r="AGD494" s="0"/>
+      <c r="AGE494" s="0"/>
+      <c r="AGF494" s="0"/>
+      <c r="AGG494" s="0"/>
+      <c r="AGH494" s="0"/>
+      <c r="AGI494" s="0"/>
+      <c r="AGJ494" s="0"/>
+      <c r="AGK494" s="0"/>
+      <c r="AGL494" s="0"/>
+      <c r="AGM494" s="0"/>
+      <c r="AGN494" s="0"/>
+      <c r="AGO494" s="0"/>
+      <c r="AGP494" s="0"/>
+      <c r="AGQ494" s="0"/>
+      <c r="AGR494" s="0"/>
+      <c r="AGS494" s="0"/>
+      <c r="AGT494" s="0"/>
+      <c r="AGU494" s="0"/>
+      <c r="AGV494" s="0"/>
+      <c r="AGW494" s="0"/>
+      <c r="AGX494" s="0"/>
+      <c r="AGY494" s="0"/>
+      <c r="AGZ494" s="0"/>
+      <c r="AHA494" s="0"/>
+      <c r="AHB494" s="0"/>
+      <c r="AHC494" s="0"/>
+      <c r="AHD494" s="0"/>
+      <c r="AHE494" s="0"/>
+      <c r="AHF494" s="0"/>
+      <c r="AHG494" s="0"/>
+      <c r="AHH494" s="0"/>
+      <c r="AHI494" s="0"/>
+      <c r="AHJ494" s="0"/>
+      <c r="AHK494" s="0"/>
+      <c r="AHL494" s="0"/>
+      <c r="AHM494" s="0"/>
+      <c r="AHN494" s="0"/>
+      <c r="AHO494" s="0"/>
+      <c r="AHP494" s="0"/>
+      <c r="AHQ494" s="0"/>
+      <c r="AHR494" s="0"/>
+      <c r="AHS494" s="0"/>
+      <c r="AHT494" s="0"/>
+      <c r="AHU494" s="0"/>
+      <c r="AHV494" s="0"/>
+      <c r="AHW494" s="0"/>
+      <c r="AHX494" s="0"/>
+      <c r="AHY494" s="0"/>
+      <c r="AHZ494" s="0"/>
+      <c r="AIA494" s="0"/>
+      <c r="AIB494" s="0"/>
+      <c r="AIC494" s="0"/>
+      <c r="AID494" s="0"/>
+      <c r="AIE494" s="0"/>
+      <c r="AIF494" s="0"/>
+      <c r="AIG494" s="0"/>
+      <c r="AIH494" s="0"/>
+      <c r="AII494" s="0"/>
+      <c r="AIJ494" s="0"/>
+      <c r="AIK494" s="0"/>
+      <c r="AIL494" s="0"/>
+      <c r="AIM494" s="0"/>
+      <c r="AIN494" s="0"/>
+      <c r="AIO494" s="0"/>
+      <c r="AIP494" s="0"/>
+      <c r="AIQ494" s="0"/>
+      <c r="AIR494" s="0"/>
+      <c r="AIS494" s="0"/>
+      <c r="AIT494" s="0"/>
+      <c r="AIU494" s="0"/>
+      <c r="AIV494" s="0"/>
+      <c r="AIW494" s="0"/>
+      <c r="AIX494" s="0"/>
+      <c r="AIY494" s="0"/>
+      <c r="AIZ494" s="0"/>
+      <c r="AJA494" s="0"/>
+      <c r="AJB494" s="0"/>
+      <c r="AJC494" s="0"/>
+      <c r="AJD494" s="0"/>
+      <c r="AJE494" s="0"/>
+      <c r="AJF494" s="0"/>
+      <c r="AJG494" s="0"/>
+      <c r="AJH494" s="0"/>
+      <c r="AJI494" s="0"/>
+      <c r="AJJ494" s="0"/>
+      <c r="AJK494" s="0"/>
+      <c r="AJL494" s="0"/>
+      <c r="AJM494" s="0"/>
+      <c r="AJN494" s="0"/>
+      <c r="AJO494" s="0"/>
+      <c r="AJP494" s="0"/>
+      <c r="AJQ494" s="0"/>
+      <c r="AJR494" s="0"/>
+      <c r="AJS494" s="0"/>
+      <c r="AJT494" s="0"/>
+      <c r="AJU494" s="0"/>
+      <c r="AJV494" s="0"/>
+      <c r="AJW494" s="0"/>
+      <c r="AJX494" s="0"/>
+      <c r="AJY494" s="0"/>
+      <c r="AJZ494" s="0"/>
+      <c r="AKA494" s="0"/>
+      <c r="AKB494" s="0"/>
+      <c r="AKC494" s="0"/>
+      <c r="AKD494" s="0"/>
+      <c r="AKE494" s="0"/>
+      <c r="AKF494" s="0"/>
+      <c r="AKG494" s="0"/>
+      <c r="AKH494" s="0"/>
+      <c r="AKI494" s="0"/>
+      <c r="AKJ494" s="0"/>
+      <c r="AKK494" s="0"/>
+      <c r="AKL494" s="0"/>
+      <c r="AKM494" s="0"/>
+      <c r="AKN494" s="0"/>
+      <c r="AKO494" s="0"/>
+      <c r="AKP494" s="0"/>
+      <c r="AKQ494" s="0"/>
+      <c r="AKR494" s="0"/>
+      <c r="AKS494" s="0"/>
+      <c r="AKT494" s="0"/>
+      <c r="AKU494" s="0"/>
+      <c r="AKV494" s="0"/>
+      <c r="AKW494" s="0"/>
+      <c r="AKX494" s="0"/>
+      <c r="AKY494" s="0"/>
+      <c r="AKZ494" s="0"/>
+      <c r="ALA494" s="0"/>
+      <c r="ALB494" s="0"/>
+      <c r="ALC494" s="0"/>
+      <c r="ALD494" s="0"/>
+      <c r="ALE494" s="0"/>
+      <c r="ALF494" s="0"/>
+      <c r="ALG494" s="0"/>
+      <c r="ALH494" s="0"/>
+      <c r="ALI494" s="0"/>
+      <c r="ALJ494" s="0"/>
+      <c r="ALK494" s="0"/>
+      <c r="ALL494" s="0"/>
+      <c r="ALM494" s="0"/>
+      <c r="ALN494" s="0"/>
+      <c r="ALO494" s="0"/>
+      <c r="ALP494" s="0"/>
+      <c r="ALQ494" s="0"/>
+      <c r="ALR494" s="0"/>
+      <c r="ALS494" s="0"/>
+      <c r="ALT494" s="0"/>
+      <c r="ALU494" s="0"/>
+      <c r="ALV494" s="0"/>
+      <c r="ALW494" s="0"/>
+      <c r="ALX494" s="0"/>
+      <c r="ALY494" s="0"/>
+      <c r="ALZ494" s="0"/>
+      <c r="AMA494" s="0"/>
+      <c r="AMB494" s="0"/>
+      <c r="AMC494" s="0"/>
+      <c r="AMD494" s="0"/>
+      <c r="AME494" s="0"/>
+      <c r="AMF494" s="0"/>
+      <c r="AMG494" s="0"/>
+      <c r="AMH494" s="0"/>
+      <c r="AMI494" s="0"/>
+      <c r="AMJ494" s="0"/>
     </row>
     <row r="495" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A495" s="24" t="s">
+      <c r="A495" s="21" t="s">
         <v>1814</v>
       </c>
       <c r="B495" s="16" t="s">
@@ -41492,17 +42470,17 @@
         <v>1817</v>
       </c>
     </row>
-    <row r="496" s="26" customFormat="true" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A496" s="25" t="s">
+    <row r="496" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A496" s="6" t="s">
         <v>1818</v>
       </c>
-      <c r="B496" s="22" t="s">
+      <c r="B496" s="16" t="s">
         <v>1819</v>
       </c>
-      <c r="C496" s="22" t="s">
+      <c r="C496" s="16" t="s">
         <v>1820</v>
       </c>
-      <c r="D496" s="22" t="s">
+      <c r="D496" s="16" t="s">
         <v>1821</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update translations for TZ Pilot
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -4884,7 +4884,7 @@
     <t xml:space="preserve">13. Este participante sofre de alguma doença crónica? (Doença de longa duração)</t>
   </si>
   <si>
-    <t xml:space="preserve">13. Mshiriki huyu kwa sasa unaugua kutokana na ugonjwa wowote sugu? (ugonjwa wa muda mrefu)</t>
+    <t xml:space="preserve">13. Mshiriki huyu anaugua ugonjwa wowote sugu kwa sasa? (ugonjwa wa muda mrefu)</t>
   </si>
   <si>
     <t xml:space="preserve">ind_q14</t>
@@ -5196,7 +5196,7 @@
     <t xml:space="preserve">31a. O que é que o participante faz?</t>
   </si>
   <si>
-    <t xml:space="preserve">31a. Mshiriki huyu anafanya nini?</t>
+    <t xml:space="preserve">31a. Ikiwa ni kabla ya  jua kuchomoza, Mshiriki huyu anafanya  nini?</t>
   </si>
   <si>
     <t xml:space="preserve">ind_q32</t>
@@ -32580,9 +32580,9 @@
   <dimension ref="A1:AMJ496"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A449" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D126" activeCellId="0" sqref="D126"/>
+      <selection pane="bottomLeft" activeCell="D469" activeCellId="0" sqref="D469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>